<commit_message>
Mudança input do modelo para produção adicional
</commit_message>
<xml_diff>
--- a/simulador_mq_v0.3.xlsx
+++ b/simulador_mq_v0.3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/yuritelles_petrobras_com_br/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/yuritelles_petrobras_com_br/Documents/Documentos/git_simulador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{A69756E9-B100-4F2F-9EF1-63B9807E025B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96340189-4021-45A0-997F-EBB2FC5610BC}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{A69756E9-B100-4F2F-9EF1-63B9807E025B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C05046-4CAA-412E-BC86-57429B0D2641}"/>
   <bookViews>
-    <workbookView xWindow="-48210" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{AAE49CED-2ACB-46D0-84E0-362A500CFA6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{AAE49CED-2ACB-46D0-84E0-362A500CFA6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Preço (US$_m3)" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,25 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
-  <si>
-    <t>p0</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Opex</t>
   </si>
@@ -114,9 +96,6 @@
     <t>Receita</t>
   </si>
   <si>
-    <t>Inclui depreciação</t>
-  </si>
-  <si>
     <t>Tributos</t>
   </si>
   <si>
@@ -137,6 +116,24 @@
   <si>
     <t>Dívida</t>
   </si>
+  <si>
+    <t>E&amp;P</t>
+  </si>
+  <si>
+    <t>Refino</t>
+  </si>
+  <si>
+    <t>Pertoquímica</t>
+  </si>
+  <si>
+    <t>Eólica</t>
+  </si>
+  <si>
+    <t>Fertilizantes</t>
+  </si>
+  <si>
+    <t>Comercialização</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +143,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +167,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,7 +243,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,6 +275,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -288,6 +296,1041 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Volume_add!$M$2:$M$27</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>41613.257139380097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41917.486089170379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42463.2120791165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43467.748810935482</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43956.664094868065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44568.001745658505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45183.736413831</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45642.672239340638</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46151.308336943614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46086.594201592503</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46642.125185254117</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47205.043941645461</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47578.40907071421</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47550.55953089735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47887.816728432816</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48229.391371569451</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46851.422747726865</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47255.901355051341</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>47710.663821630136</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>48052.361957946967</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>48612.43184207016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49399.13199333605</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48560.072881118052</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>49278.076062902772</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49776.262644665738</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50463.218532070612</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5873-40B4-B95B-FD22FF571635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Volume_add!$N$2:$N$27</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>41613.257139380097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44094.903152191888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46818.04620515951</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50488.915283932583</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51100.252934723023</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51715.987602895519</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52174.923428405156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52683.559526008132</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52618.845390657021</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53174.376374318635</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53737.295130709979</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54110.660259778728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>54082.810719961868</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>54420.067917497334</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>54761.642560633969</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53383.673936791383</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>53788.152544115859</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54242.915010694654</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54584.613147011485</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55144.683031134678</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>55931.383182400568</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55092.324070182571</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>55810.32725196729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>56308.513833730256</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56995.46972113513</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5873-40B4-B95B-FD22FF571635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1605619072"/>
+        <c:axId val="1597335536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1605619072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1597335536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1597335536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1605619072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76933</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>115765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>399317</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A5609CD-5DC0-432E-F5B3-67525CA8BE99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -589,7 +1632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1482F7EC-D512-4D3C-A0E5-D86E3932F98F}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -599,22 +1644,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1237,23 +2282,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="str" cm="1">
+        <f t="array" ref="B1:G1">'Preço (US$_m3)'!B1:G1</f>
+        <v>E&amp;P</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Refino</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Comercialização</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>Pertoquímica</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>Eólica</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>Fertilizantes</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,23 +2921,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="str" cm="1">
+        <f t="array" ref="B1:G1">'Preço (US$_m3)'!B1:G1</f>
+        <v>E&amp;P</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Refino</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Comercialização</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>Pertoquímica</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>Eólica</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>Fertilizantes</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,13 +3560,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2893,40 +3940,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA401CBF-3FE6-418D-810B-8FDA9D905A6D}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="2"/>
     <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="7.7109375" style="1"/>
+    <col min="3" max="3" width="7.7109375" style="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.7109375" style="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="1"/>
+    <col min="11" max="11" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="7.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="str" cm="1">
+        <f t="array" ref="B1:G1">'Preço (US$_m3)'!B1:G1</f>
+        <v>E&amp;P</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Refino</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Comercialização</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>Pertoquímica</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>Eólica</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>Fertilizantes</v>
+      </c>
+      <c r="I1" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J1" s="1">
+        <f>_xlfn.XLOOKUP(Sim!B12,'Volume (mil m3)'!$A$2:$A$27,'Volume (mil m3)'!$B$2:$B$27)</f>
+        <v>43467.748810935482</v>
+      </c>
+      <c r="K1" s="5">
+        <f>I1-J1</f>
+        <v>6532.2511890645183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2025</v>
       </c>
@@ -2954,8 +4020,24 @@
         <f t="array" ref="G2:G27">_xlfn.LET(_xlpm.x,($A2:$A27-Sim!G11)/(Sim!G12-Sim!G11),(_xlpm.x&gt;1)*(1-_xlpm.x)+(_xlpm.x&gt;0)*_xlpm.x)*(Sim!G10-Sim!G9)*'Demanda (mil m3)'!G2:G27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="5" cm="1">
+        <f t="array" ref="K2:K27">_xlfn.LET(_xlpm.x,($A2:$A27-Sim!B11)/(Sim!B12-Sim!B11),(_xlpm.x&gt;1)*(1-_xlpm.x)+(_xlpm.x&gt;0)*_xlpm.x)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" cm="1">
+        <f t="array" ref="L2:L27">_xlfn.ANCHORARRAY(K2)*_xlfn.ANCHORARRAY(K1)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" cm="1">
+        <f t="array" ref="M2:M27">'Volume (mil m3)'!B2:B27</f>
+        <v>41613.257139380097</v>
+      </c>
+      <c r="N2" s="5" cm="1">
+        <f t="array" ref="N2:N27">_xlfn.ANCHORARRAY(M2)+_xlfn.ANCHORARRAY(L2)</f>
+        <v>41613.257139380097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2026</v>
       </c>
@@ -2977,8 +4059,21 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+      <c r="K3" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2177.4170630215058</v>
+      </c>
+      <c r="M3" s="5">
+        <v>41917.486089170379</v>
+      </c>
+      <c r="N3" s="5">
+        <v>44094.903152191888</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2027</v>
       </c>
@@ -3000,8 +4095,21 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+      <c r="K4" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L4" s="5">
+        <v>4354.8341260430116</v>
+      </c>
+      <c r="M4" s="5">
+        <v>42463.2120791165</v>
+      </c>
+      <c r="N4" s="5">
+        <v>46818.04620515951</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2028</v>
       </c>
@@ -3023,8 +4131,21 @@
       <c r="G5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M5" s="5">
+        <v>43467.748810935482</v>
+      </c>
+      <c r="N5" s="5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2029</v>
       </c>
@@ -3046,8 +4167,21 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="5"/>
+      <c r="K6" s="5">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M6" s="5">
+        <v>43956.664094868065</v>
+      </c>
+      <c r="N6" s="5">
+        <v>50488.915283932583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2030</v>
       </c>
@@ -3069,8 +4203,21 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M7" s="5">
+        <v>44568.001745658505</v>
+      </c>
+      <c r="N7" s="5">
+        <v>51100.252934723023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2031</v>
       </c>
@@ -3087,13 +4234,26 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>219.39655791826817</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="5"/>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M8" s="5">
+        <v>45183.736413831</v>
+      </c>
+      <c r="N8" s="5">
+        <v>51715.987602895519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2032</v>
       </c>
@@ -3110,13 +4270,26 @@
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>448.76504885786483</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M9" s="5">
+        <v>45642.672239340638</v>
+      </c>
+      <c r="N9" s="5">
+        <v>52174.923428405156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2033</v>
       </c>
@@ -3133,13 +4306,26 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>633.05359545405327</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+      <c r="K10" s="5">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M10" s="5">
+        <v>46151.308336943614</v>
+      </c>
+      <c r="N10" s="5">
+        <v>52683.559526008132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2034</v>
       </c>
@@ -3156,13 +4342,26 @@
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>811.79310472975021</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="5"/>
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M11" s="5">
+        <v>46086.594201592503</v>
+      </c>
+      <c r="N11" s="5">
+        <v>52618.845390657021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2035</v>
       </c>
@@ -3179,13 +4378,26 @@
         <v>0</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>967.53530157047783</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M12" s="5">
+        <v>46642.125185254117</v>
+      </c>
+      <c r="N12" s="5">
+        <v>53174.376374318635</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2036</v>
       </c>
@@ -3202,13 +4414,26 @@
         <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>934.20370723668043</v>
       </c>
       <c r="G13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M13" s="5">
+        <v>47205.043941645461</v>
+      </c>
+      <c r="N13" s="5">
+        <v>53737.295130709979</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2037</v>
       </c>
@@ -3225,13 +4450,26 @@
         <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>900.12205613869094</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="5"/>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M14" s="5">
+        <v>47578.40907071421</v>
+      </c>
+      <c r="N14" s="5">
+        <v>54110.660259778728</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2038</v>
       </c>
@@ -3248,13 +4486,26 @@
         <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>218.97213271163469</v>
+        <v>875.88853084653874</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="5"/>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+      <c r="L15" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M15" s="5">
+        <v>47550.55953089735</v>
+      </c>
+      <c r="N15" s="5">
+        <v>54082.810719961868</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2039</v>
       </c>
@@ -3271,13 +4522,26 @@
         <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>426.8187702273957</v>
+        <v>853.63754045479141</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="5"/>
+      <c r="K16" s="5">
+        <v>1</v>
+      </c>
+      <c r="L16" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M16" s="5">
+        <v>47887.816728432816</v>
+      </c>
+      <c r="N16" s="5">
+        <v>54420.067917497334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2040</v>
       </c>
@@ -3294,13 +4558,26 @@
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>627.58646361564502</v>
+        <v>836.78195148752673</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="5"/>
+      <c r="K17" s="5">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M17" s="5">
+        <v>48229.391371569451</v>
+      </c>
+      <c r="N17" s="5">
+        <v>54761.642560633969</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2041</v>
       </c>
@@ -3322,8 +4599,21 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="5"/>
+      <c r="K18" s="5">
+        <v>1</v>
+      </c>
+      <c r="L18" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M18" s="5">
+        <v>46851.422747726865</v>
+      </c>
+      <c r="N18" s="5">
+        <v>53383.673936791383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2042</v>
       </c>
@@ -3345,8 +4635,21 @@
       <c r="G19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="5"/>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M19" s="5">
+        <v>47255.901355051341</v>
+      </c>
+      <c r="N19" s="5">
+        <v>53788.152544115859</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2043</v>
       </c>
@@ -3368,8 +4671,21 @@
       <c r="G20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="5"/>
+      <c r="K20" s="5">
+        <v>1</v>
+      </c>
+      <c r="L20" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M20" s="5">
+        <v>47710.663821630136</v>
+      </c>
+      <c r="N20" s="5">
+        <v>54242.915010694654</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2044</v>
       </c>
@@ -3391,8 +4707,21 @@
       <c r="G21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="5"/>
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
+      <c r="L21" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M21" s="5">
+        <v>48052.361957946967</v>
+      </c>
+      <c r="N21" s="5">
+        <v>54584.613147011485</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2045</v>
       </c>
@@ -3414,8 +4743,21 @@
       <c r="G22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="5"/>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M22" s="5">
+        <v>48612.43184207016</v>
+      </c>
+      <c r="N22" s="5">
+        <v>55144.683031134678</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2046</v>
       </c>
@@ -3437,8 +4779,21 @@
       <c r="G23" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="5"/>
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+      <c r="L23" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M23" s="5">
+        <v>49399.13199333605</v>
+      </c>
+      <c r="N23" s="5">
+        <v>55931.383182400568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2047</v>
       </c>
@@ -3460,8 +4815,21 @@
       <c r="G24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="5"/>
+      <c r="K24" s="5">
+        <v>1</v>
+      </c>
+      <c r="L24" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M24" s="5">
+        <v>48560.072881118052</v>
+      </c>
+      <c r="N24" s="5">
+        <v>55092.324070182571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2048</v>
       </c>
@@ -3483,8 +4851,21 @@
       <c r="G25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="5"/>
+      <c r="K25" s="5">
+        <v>1</v>
+      </c>
+      <c r="L25" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M25" s="5">
+        <v>49278.076062902772</v>
+      </c>
+      <c r="N25" s="5">
+        <v>55810.32725196729</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2049</v>
       </c>
@@ -3506,8 +4887,21 @@
       <c r="G26" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="5"/>
+      <c r="K26" s="5">
+        <v>1</v>
+      </c>
+      <c r="L26" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M26" s="5">
+        <v>49776.262644665738</v>
+      </c>
+      <c r="N26" s="5">
+        <v>56308.513833730256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2050</v>
       </c>
@@ -3528,6 +4922,19 @@
       </c>
       <c r="G27" s="4">
         <v>0</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="K27" s="5">
+        <v>1</v>
+      </c>
+      <c r="L27" s="5">
+        <v>6532.2511890645183</v>
+      </c>
+      <c r="M27" s="5">
+        <v>50463.218532070612</v>
+      </c>
+      <c r="N27" s="5">
+        <v>56995.46972113513</v>
       </c>
     </row>
   </sheetData>
@@ -3535,6 +4942,7 @@
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Trebuchet MS"&amp;9&amp;K737373 PÚBLICA</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3542,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082DEB08-9530-4F78-84F1-21D50050C17D}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3553,28 +4961,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="str" cm="1">
+        <f t="array" ref="B1:G1">'Preço (US$_m3)'!B1:G1</f>
+        <v>E&amp;P</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Refino</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Comercialização</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>Pertoquímica</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>Eólica</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>Fertilizantes</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="6">
         <v>278.61022865490668</v>
@@ -3594,13 +5003,11 @@
       <c r="G2" s="6">
         <v>279.45612042703505</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6">
         <v>83.583068596472003</v>
@@ -3620,10 +5027,11 @@
       <c r="G3" s="6">
         <v>83.836836128110505</v>
       </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" s="7">
         <v>5</v>
@@ -3646,7 +5054,7 @@
     </row>
     <row r="5" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
         <v>5</v>
@@ -3669,7 +5077,7 @@
     </row>
     <row r="6" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
         <v>0.1</v>
@@ -3692,7 +5100,7 @@
     </row>
     <row r="7" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
         <v>0.34</v>
@@ -3715,7 +5123,7 @@
     </row>
     <row r="9" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" cm="1">
         <f t="array" ref="B9">AVERAGE('Volume (mil m3)'!B2:B27/'Demanda (mil m3)'!B2:B27)</f>
@@ -3744,7 +5152,7 @@
     </row>
     <row r="10" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" s="9">
         <v>0.9</v>
@@ -3767,7 +5175,7 @@
     </row>
     <row r="11" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="10">
         <v>2025</v>
@@ -3782,7 +5190,7 @@
         <v>2038</v>
       </c>
       <c r="F11" s="10">
-        <v>2037</v>
+        <v>2030</v>
       </c>
       <c r="G11" s="10">
         <v>2030</v>
@@ -3790,7 +5198,7 @@
     </row>
     <row r="12" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B12" s="10">
         <v>2028</v>
@@ -3805,7 +5213,8 @@
         <v>2043</v>
       </c>
       <c r="F12" s="10">
-        <v>2041</v>
+        <f>F11+5</f>
+        <v>2035</v>
       </c>
       <c r="G12" s="10">
         <v>2035</v>
@@ -3823,8 +5232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4650035-0809-4929-BA00-4DCC0C21969B}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3835,26 +5244,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>